<commit_message>
provide some instructions & example on how to use leave import template
</commit_message>
<xml_diff>
--- a/templates/accupay-leave-template.xlsx
+++ b/templates/accupay-leave-template.xlsx
@@ -4,17 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="309"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="527"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
+    <sheet name="R E A D  M E  F I R S T" sheetId="5" r:id="rId2"/>
+    <sheet name="E  X  A  M  P  L  E" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
   <si>
     <t>Employee ID</t>
   </si>
@@ -25,12 +27,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Start Time</t>
-  </si>
-  <si>
-    <t>End Time</t>
-  </si>
-  <si>
     <t>Start Date</t>
   </si>
   <si>
@@ -41,6 +37,78 @@
   </si>
   <si>
     <t>Comment</t>
+  </si>
+  <si>
+    <t>AccuPay Leave Import Template</t>
+  </si>
+  <si>
+    <t>Using this file, you can simply import a few or a bunch of employees' filed leaves. List below are columns you need to supply information.</t>
+  </si>
+  <si>
+    <t>Column</t>
+  </si>
+  <si>
+    <t>Desciption</t>
+  </si>
+  <si>
+    <t>the company's provided ID for the employee</t>
+  </si>
+  <si>
+    <t>the type of leave that the employee desired to use</t>
+  </si>
+  <si>
+    <t>detemines whether the user grants the leave or not</t>
+  </si>
+  <si>
+    <t>Start Time (Optional)</t>
+  </si>
+  <si>
+    <t>End Time (Optional)</t>
+  </si>
+  <si>
+    <t>the date when the filed leave begins</t>
+  </si>
+  <si>
+    <t>the explanation or notes why employee uses leave</t>
+  </si>
+  <si>
+    <t>user can add comments with regards to this matter</t>
+  </si>
+  <si>
+    <t>NOTE :</t>
+  </si>
+  <si>
+    <t>worksheet name could be what ever the user desires</t>
+  </si>
+  <si>
+    <t>refer to the `E  X  A  M  P  L  E` worksheet</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>Vacation leave</t>
+  </si>
+  <si>
+    <t>Approved</t>
+  </si>
+  <si>
+    <t>Sick Leave</t>
+  </si>
+  <si>
+    <t>Family vacation</t>
+  </si>
+  <si>
+    <t>not feeling well</t>
+  </si>
+  <si>
+    <t>the time when the filed leave begins. Leave it blank as long the user already provided the shift schedule in AccuPay</t>
+  </si>
+  <si>
+    <t>the time when the filed leave ends. Leave it blank as long the user already provided the shift schedule in AccuPay</t>
+  </si>
+  <si>
+    <t>the date when the filed leave ends. Leave it blank if value is the same as `Start Date`</t>
   </si>
 </sst>
 </file>
@@ -51,12 +119,19 @@
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -69,6 +144,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -94,9 +176,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
@@ -110,9 +192,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma 2" xfId="1"/>
@@ -441,16 +535,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" style="1" customWidth="1"/>
-    <col min="4" max="5" width="14.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.42578125" style="2" customWidth="1"/>
     <col min="7" max="7" width="21.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="32.5703125" style="1" customWidth="1"/>
@@ -472,27 +565,27 @@
         <v>2</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="G1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="H1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="I1" s="5" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection password="CD03" sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0"/>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576">
       <formula1>"Leave w/o Pay,Maternity/paternity leave,Others,Sick leave,Vacation leave,Additional VL"</formula1>
     </dataValidation>
@@ -503,4 +596,238 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23" style="10" customWidth="1"/>
+    <col min="2" max="2" width="105.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="26.25">
+      <c r="A1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="9"/>
+    </row>
+    <row r="3" spans="1:2" ht="32.25" customHeight="1">
+      <c r="A3" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="11"/>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection password="CD03" sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A3:B3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.85546875" customWidth="1"/>
+    <col min="9" max="9" width="26.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="15">
+        <f ca="1">TODAY()+(7-WEEKDAY(TODAY(),2)+1)</f>
+        <v>43563</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="15">
+        <f ca="1">TODAY()+(7-WEEKDAY(TODAY(),2)+2)</f>
+        <v>43564</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection password="CD03" sheet="1" objects="1" scenarios="1"/>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1">
+      <formula1>"Pending,Approved"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>"Leave w/o Pay,Maternity/paternity leave,Others,Sick leave,Vacation leave,Additional VL"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>